<commit_message>
Command Module Pricing, EntryCosts, Tech Requirements
* Command Modules from Vostok and Mercury through Apollo have been properly costed and set proper entryCosts
* Some CM's have moved into earlier nodes to fit with the technology of the time even though they flew later
* Soyuz needs another pass and I will be looking at that next.
</commit_message>
<xml_diff>
--- a/Notes/Pricing/CapsulePricing.xlsx
+++ b/Notes/Pricing/CapsulePricing.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pap\Dropbox\GAMES\KSP\Git\RP-0\Notes\Pricing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4ADB3A5C-0666-4C81-8F7E-2ED1F0BA47D9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598906CE-1B2A-4E5D-BE1B-87713E748239}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11925" xr2:uid="{FD47FD07-80A1-481C-B017-802BD41F3547}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11925" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="136">
   <si>
     <t>Spacecraft</t>
   </si>
@@ -264,13 +264,178 @@
     <t>ECM's</t>
   </si>
   <si>
-    <t>Apollo (CM/SM)</t>
-  </si>
-  <si>
-    <t>Gemini (CM/SM)</t>
-  </si>
-  <si>
-    <t>capsulesBasic, heatshieldsLEO</t>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>basicCapsules</t>
+  </si>
+  <si>
+    <t>secondGenCapsules</t>
+  </si>
+  <si>
+    <t>Gemini CM</t>
+  </si>
+  <si>
+    <t>Gemini SM</t>
+  </si>
+  <si>
+    <t>Apollo CM</t>
+  </si>
+  <si>
+    <t>Apollo SM</t>
+  </si>
+  <si>
+    <t>matureCapsules</t>
+  </si>
+  <si>
+    <t>7K-OK CM</t>
+  </si>
+  <si>
+    <t>7K-OK-SM</t>
+  </si>
+  <si>
+    <t>Big G</t>
+  </si>
+  <si>
+    <t>VA Capsule</t>
+  </si>
+  <si>
+    <t>7K-LOK CM</t>
+  </si>
+  <si>
+    <t>Vostok SM</t>
+  </si>
+  <si>
+    <t>Voskhod Airlock</t>
+  </si>
+  <si>
+    <t>Voskhod Total</t>
+  </si>
+  <si>
+    <t>Voskhod Capsule</t>
+  </si>
+  <si>
+    <t>7K-L1</t>
+  </si>
+  <si>
+    <t>7K-LOK SM</t>
+  </si>
+  <si>
+    <t>TK-T CM</t>
+  </si>
+  <si>
+    <t>TK-T SM</t>
+  </si>
+  <si>
+    <t>capsulesBasic, capsulesAirlock</t>
+  </si>
+  <si>
+    <t>capsulesBasic, VostokSM</t>
+  </si>
+  <si>
+    <t>Vostok Total</t>
+  </si>
+  <si>
+    <t>Gemini Total</t>
+  </si>
+  <si>
+    <t>Vostok Capsule</t>
+  </si>
+  <si>
+    <t>7K-OK Total</t>
+  </si>
+  <si>
+    <t>40000, capsulesBasic</t>
+  </si>
+  <si>
+    <t>6000, capsulesBasic</t>
+  </si>
+  <si>
+    <t>18000</t>
+  </si>
+  <si>
+    <t>capsulesSecondGen, capsulesAirlock, capsulesBasic</t>
+  </si>
+  <si>
+    <t>80000</t>
+  </si>
+  <si>
+    <t>15000, capsulesBasic</t>
+  </si>
+  <si>
+    <t>25000, capsulesSecondGen, capsulesAirlock</t>
+  </si>
+  <si>
+    <t>100000, VostokSM</t>
+  </si>
+  <si>
+    <t>capsulesMature, heatshieldsLunar</t>
+  </si>
+  <si>
+    <t>115000, capsulesGemini</t>
+  </si>
+  <si>
+    <t>100000, capsulesMature</t>
+  </si>
+  <si>
+    <t>30000, 7KOKSM, VostokSM</t>
+  </si>
+  <si>
+    <t>Family</t>
+  </si>
+  <si>
+    <t>Vostok</t>
+  </si>
+  <si>
+    <t>Gemini</t>
+  </si>
+  <si>
+    <t>Apollo</t>
+  </si>
+  <si>
+    <t>Soyuz</t>
+  </si>
+  <si>
+    <t>TKS</t>
+  </si>
+  <si>
+    <t>capsulesSoyuz</t>
+  </si>
+  <si>
+    <t>capsulesSoyuz, heatshieldsLunar</t>
+  </si>
+  <si>
+    <t>140000, capsulesSoyuz, heatshieldsLunar</t>
+  </si>
+  <si>
+    <t>100000, capsulesSoyuz, heatshieldsLunar</t>
+  </si>
+  <si>
+    <t>100000, capsulesSoyuz</t>
+  </si>
+  <si>
+    <t>entryCost Soyuz unlocked</t>
+  </si>
+  <si>
+    <t>Apollo Total</t>
+  </si>
+  <si>
+    <t>7K-LOK Total</t>
+  </si>
+  <si>
+    <t>TK-T Total</t>
+  </si>
+  <si>
+    <t>capsulesMercury, capsulesSecondGen, capsulesAirlock</t>
+  </si>
+  <si>
+    <t>100000, capsulesMercury, capsulesSecondGen, capsulesAirlock</t>
+  </si>
+  <si>
+    <t>170000, GeminiSM</t>
+  </si>
+  <si>
+    <t>500000, capsulesMature, heatshieldsLunar</t>
   </si>
 </sst>
 </file>
@@ -281,7 +446,14 @@
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,12 +462,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -307,10 +491,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -323,11 +508,51 @@
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="6" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="6" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="10" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -338,6 +563,23 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:H26" totalsRowShown="0" dataDxfId="4">
+  <autoFilter ref="A1:H26" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Spacecraft"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Level"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Family"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Cost" dataDxfId="3"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Total entryCost" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Actual entryCost" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="entryCost Soyuz unlocked" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="ECM's"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -636,244 +878,822 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4D4980B-DB89-4488-BDA9-26725078DE04}">
-  <dimension ref="A1:E37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" customWidth="1"/>
+    <col min="8" max="8" width="56.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" t="s">
         <v>74</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>75</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>76</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7">
         <v>2468</v>
       </c>
-      <c r="C2" s="3">
+      <c r="E2" s="7">
         <v>100000</v>
       </c>
-      <c r="D2" s="3">
+      <c r="F2" s="7">
         <v>80000</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" s="7"/>
+      <c r="H2" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="7">
+        <f>1600+650</f>
+        <v>2250</v>
+      </c>
+      <c r="E3" s="7">
+        <v>84000</v>
+      </c>
+      <c r="F3" s="7">
+        <v>64000</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1600</v>
+      </c>
+      <c r="E4" s="7">
+        <f>E3-18000</f>
+        <v>66000</v>
+      </c>
+      <c r="F4" s="7">
+        <v>46000</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="H4" s="6" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="7">
+        <v>650</v>
+      </c>
+      <c r="E5" s="7">
+        <v>18000</v>
+      </c>
+      <c r="F5" s="7">
+        <v>18000</v>
+      </c>
+      <c r="G5" s="7"/>
+      <c r="H5" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
+      <c r="C6" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="7">
+        <v>13000</v>
+      </c>
+      <c r="E6" s="7">
+        <v>560000</v>
+      </c>
+      <c r="F6" s="7">
+        <v>500000</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="H6" s="6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D7" s="7">
+        <v>9000</v>
+      </c>
+      <c r="E7" s="7">
+        <v>480000</v>
+      </c>
+      <c r="F7" s="7">
+        <v>420000</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="6" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" s="7">
+        <v>4000</v>
+      </c>
+      <c r="E8" s="7">
+        <v>80000</v>
+      </c>
+      <c r="F8" s="7">
+        <v>80000</v>
+      </c>
+      <c r="G8" s="7"/>
+      <c r="H8" s="8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" s="7">
+        <v>3000</v>
+      </c>
+      <c r="E9" s="7">
+        <v>125000</v>
+      </c>
+      <c r="F9" s="7">
+        <v>65000</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D10" s="7">
+        <v>2000</v>
+      </c>
+      <c r="E10" s="7">
+        <v>75000</v>
+      </c>
+      <c r="F10" s="7">
+        <v>15000</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="H10" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" s="7">
+        <v>1000</v>
+      </c>
+      <c r="E11" s="7">
+        <v>50000</v>
+      </c>
+      <c r="F11" s="7">
+        <v>50000</v>
+      </c>
+      <c r="G11" s="7"/>
+      <c r="H11" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D12" s="11">
+        <v>12000</v>
+      </c>
+      <c r="E12" s="11">
+        <v>478000</v>
+      </c>
+      <c r="F12" s="11">
+        <v>400000</v>
+      </c>
+      <c r="G12" s="11"/>
+      <c r="H12" s="10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D13" s="11">
+        <v>8400</v>
+      </c>
+      <c r="E13" s="11">
+        <v>360000</v>
+      </c>
+      <c r="F13" s="11">
+        <v>300000</v>
+      </c>
+      <c r="G13" s="11"/>
+      <c r="H13" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="D14" s="11">
+        <v>3600</v>
+      </c>
+      <c r="E14" s="11">
+        <v>118000</v>
+      </c>
+      <c r="F14" s="11">
+        <v>100000</v>
+      </c>
+      <c r="G14" s="11"/>
+      <c r="H14" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15" s="13">
+        <v>44000</v>
+      </c>
+      <c r="E15" s="14">
+        <v>1415000</v>
+      </c>
+      <c r="F15" s="13">
+        <v>1000000</v>
+      </c>
+      <c r="G15" s="13"/>
+      <c r="H15" s="12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D16" s="13">
+        <v>35000</v>
+      </c>
+      <c r="E16" s="13">
+        <f>985000+180000</f>
+        <v>1165000</v>
+      </c>
+      <c r="F16" s="13">
+        <f>650000+180000</f>
+        <v>830000</v>
+      </c>
+      <c r="G16" s="13"/>
+      <c r="H16" s="12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17" s="13">
+        <v>9000</v>
+      </c>
+      <c r="E17" s="13">
+        <f>430000-180000</f>
+        <v>250000</v>
+      </c>
+      <c r="F17" s="13">
+        <v>170000</v>
+      </c>
+      <c r="G17" s="13"/>
+      <c r="H17" s="12" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="D18" s="13">
+        <v>12000</v>
+      </c>
+      <c r="E18" s="13">
+        <f>115000+500000</f>
+        <v>615000</v>
+      </c>
+      <c r="F18" s="13">
+        <v>115000</v>
+      </c>
+      <c r="G18" s="13"/>
+      <c r="H18" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="K18">
+        <f>320000-500000</f>
+        <v>-180000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" t="s">
+        <v>122</v>
+      </c>
+      <c r="D19" s="3">
+        <v>8000</v>
+      </c>
+      <c r="E19" s="3">
+        <v>735000</v>
+      </c>
+      <c r="F19" s="3">
+        <v>400000</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" t="s">
+        <v>115</v>
+      </c>
+      <c r="K19">
+        <f>350000+K18</f>
+        <v>170000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>130</v>
+      </c>
+      <c r="B20" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" t="s">
+        <v>121</v>
+      </c>
+      <c r="D20" s="3">
+        <v>24000</v>
+      </c>
+      <c r="E20" s="3">
+        <v>923000</v>
+      </c>
+      <c r="F20" s="3">
+        <v>500000</v>
+      </c>
+      <c r="G20" s="3">
+        <v>200000</v>
+      </c>
+      <c r="H20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" t="s">
+        <v>121</v>
+      </c>
+      <c r="D21" s="3">
+        <v>17000</v>
+      </c>
+      <c r="E21" s="3">
+        <v>775000</v>
+      </c>
+      <c r="F21" s="3">
+        <v>470000</v>
+      </c>
+      <c r="G21" s="3">
+        <v>170000</v>
+      </c>
+      <c r="H21" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" t="s">
+        <v>121</v>
+      </c>
+      <c r="D22" s="3">
+        <v>7000</v>
+      </c>
+      <c r="E22" s="3">
+        <v>148000</v>
+      </c>
+      <c r="F22" s="3">
+        <v>30000</v>
+      </c>
+      <c r="G22" s="3">
+        <v>30000</v>
+      </c>
+      <c r="H22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>95</v>
+      </c>
+      <c r="B23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" t="s">
+        <v>121</v>
+      </c>
+      <c r="D23" s="3">
+        <v>12000</v>
+      </c>
+      <c r="E23" s="3">
+        <v>765000</v>
+      </c>
+      <c r="F23" s="3">
+        <v>430000</v>
+      </c>
+      <c r="G23" s="3">
+        <v>130000</v>
+      </c>
+      <c r="H23" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>131</v>
+      </c>
+      <c r="B24" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" t="s">
+        <v>121</v>
+      </c>
+      <c r="D24" s="3">
+        <v>15000</v>
+      </c>
+      <c r="E24" s="3">
+        <v>883000</v>
+      </c>
+      <c r="F24" s="3">
+        <v>430000</v>
+      </c>
+      <c r="G24" s="3">
+        <v>130000</v>
+      </c>
+      <c r="H24" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" t="s">
+        <v>121</v>
+      </c>
+      <c r="D25" s="3">
+        <v>11000</v>
+      </c>
+      <c r="E25" s="3">
+        <v>735000</v>
+      </c>
+      <c r="F25" s="3">
+        <v>400000</v>
+      </c>
+      <c r="G25" s="3">
+        <v>100000</v>
+      </c>
+      <c r="H25" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>98</v>
+      </c>
+      <c r="B26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" t="s">
+        <v>121</v>
+      </c>
+      <c r="D26" s="3">
+        <v>4000</v>
+      </c>
+      <c r="E26" s="3">
+        <v>148000</v>
+      </c>
+      <c r="F26" s="3">
+        <v>30000</v>
+      </c>
+      <c r="G26" s="3">
+        <v>30000</v>
+      </c>
+      <c r="H26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D27" s="3"/>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D28" s="3"/>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D30" s="3"/>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D31" s="9">
+        <f>15*0.7</f>
+        <v>10.5</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D32" s="3"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D33" s="3"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D34" s="3"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+    </row>
+    <row r="35" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D35" s="3"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D36" s="3"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+    </row>
+    <row r="37" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="3"/>
+    </row>
+    <row r="38" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+    </row>
+    <row r="39" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D39" s="3"/>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+    </row>
+    <row r="40" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+    </row>
+    <row r="41" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+    </row>
+    <row r="42" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D42" s="3"/>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+    </row>
+    <row r="43" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+    </row>
+    <row r="44" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+    </row>
+    <row r="45" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+    </row>
+    <row r="46" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+    </row>
+    <row r="47" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6771EAF3-8F97-49AA-BD54-E4D389D4C7A5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H14"/>
   <sheetViews>
@@ -1101,12 +1921,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA0B8DDC-4FC8-40A6-B466-B12ACBD98900}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:C16"/>
+      <selection activeCell="H2" sqref="E2:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1427,7 +2247,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A0A79FB-00DF-4F69-80EE-9C431A2D424B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:M31"/>
   <sheetViews>

</xml_diff>